<commit_message>
hola mundo con DIOS!!!!!!
</commit_message>
<xml_diff>
--- a/core/media/Plantilla_ejemplo.xlsx
+++ b/core/media/Plantilla_ejemplo.xlsx
@@ -591,9 +591,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="5.0"/>
     <col customWidth="1" min="2" max="2" width="6.86"/>
-    <col customWidth="1" min="3" max="3" width="8.57"/>
-    <col customWidth="1" min="4" max="4" width="5.43"/>
-    <col customWidth="1" min="5" max="5" width="8.57"/>
+    <col customWidth="1" min="3" max="5" width="8.57"/>
     <col customWidth="1" min="6" max="6" width="3.71"/>
     <col customWidth="1" min="7" max="7" width="5.43"/>
     <col customWidth="1" min="8" max="8" width="11.86"/>
@@ -608,13 +606,14 @@
     <col customWidth="1" min="21" max="21" width="4.29"/>
     <col customWidth="1" min="22" max="22" width="12.43"/>
     <col customWidth="1" min="23" max="23" width="5.0"/>
-    <col customWidth="1" min="24" max="24" width="6.29"/>
-    <col customWidth="1" min="25" max="25" width="4.57"/>
+    <col customWidth="1" min="24" max="24" width="8.0"/>
+    <col customWidth="1" min="25" max="25" width="8.71"/>
     <col customWidth="1" min="26" max="26" width="10.43"/>
     <col customWidth="1" min="27" max="27" width="9.71"/>
     <col customWidth="1" min="28" max="28" width="16.43"/>
     <col customWidth="1" min="29" max="29" width="13.29"/>
-    <col customWidth="1" min="30" max="31" width="10.71"/>
+    <col customWidth="1" min="30" max="30" width="15.0"/>
+    <col customWidth="1" min="31" max="31" width="10.71"/>
     <col customWidth="1" min="32" max="32" width="17.57"/>
     <col customWidth="1" min="33" max="37" width="10.71"/>
   </cols>
@@ -1977,7 +1976,7 @@
         <v>59.46</v>
       </c>
       <c r="Y13" s="15">
-        <v>25195.0</v>
+        <v>25.19</v>
       </c>
       <c r="Z13" s="2" t="s">
         <v>63</v>
@@ -2084,7 +2083,7 @@
         <v>37.458</v>
       </c>
       <c r="Y14" s="15">
-        <v>15872.0</v>
+        <v>15.87</v>
       </c>
       <c r="Z14" s="2" t="s">
         <v>63</v>
@@ -2191,7 +2190,7 @@
         <v>35.676</v>
       </c>
       <c r="Y15" s="15">
-        <v>15117.0</v>
+        <v>15.11</v>
       </c>
       <c r="Z15" s="2" t="s">
         <v>63</v>
@@ -2298,7 +2297,7 @@
         <v>12.486</v>
       </c>
       <c r="Y16" s="15">
-        <v>5291.0</v>
+        <v>52.91</v>
       </c>
       <c r="Z16" s="2" t="s">
         <v>63</v>
@@ -2405,7 +2404,7 @@
         <v>26.63</v>
       </c>
       <c r="Y17" s="6">
-        <v>11284.0</v>
+        <v>11.284</v>
       </c>
       <c r="Z17" s="2" t="s">
         <v>41</v>
@@ -2512,7 +2511,7 @@
         <v>52.825</v>
       </c>
       <c r="Y18" s="6">
-        <v>22383.0</v>
+        <v>22.383</v>
       </c>
       <c r="Z18" s="2" t="s">
         <v>41</v>

</xml_diff>